<commit_message>
service card & report layout changes
</commit_message>
<xml_diff>
--- a/tmp/quarterlyReport.xlsx
+++ b/tmp/quarterlyReport.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038FE7BE-74CB-4BB7-8C8C-D45C666084B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -295,31 +294,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>1043940</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1238250</xdr:rowOff>
+      <xdr:rowOff>1234440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784F8431-86D4-4ED5-BF7A-BE7D5693031A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -332,8 +325,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="552450" y="38100"/>
-          <a:ext cx="2847975" cy="1200150"/>
+          <a:off x="1043940" y="0"/>
+          <a:ext cx="2484120" cy="1234440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -666,25 +659,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -695,7 +688,7 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
@@ -706,7 +699,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -729,7 +722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="8"/>
       <c r="C4" s="4"/>
@@ -738,7 +731,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="8"/>
       <c r="C5" s="4"/>
@@ -747,7 +740,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="8"/>
       <c r="C6" s="4"/>
@@ -756,7 +749,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="8"/>
       <c r="C7" s="4"/>
@@ -765,7 +758,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="8"/>
       <c r="C8" s="4"/>
@@ -774,7 +767,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="8"/>
       <c r="C9" s="4"/>
@@ -783,7 +776,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="8"/>
       <c r="C10" s="4"/>
@@ -792,7 +785,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="8"/>
       <c r="C11" s="4"/>
@@ -801,7 +794,7 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="8"/>
       <c r="C12" s="4"/>
@@ -810,7 +803,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="8"/>
       <c r="C13" s="4"/>
@@ -819,7 +812,7 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="8"/>
       <c r="C14" s="4"/>
@@ -828,7 +821,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="8"/>
       <c r="C15" s="4"/>

</xml_diff>

<commit_message>
service dates added in monthly report
</commit_message>
<xml_diff>
--- a/tmp/quarterlyReport.xlsx
+++ b/tmp/quarterlyReport.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA16F017-1A11-4B6B-A238-7F82EBF057C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCA5883-5029-4EBD-A9BE-07D17BCC9C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,12 +24,6 @@
   </si>
   <si>
     <t>Service Type</t>
-  </si>
-  <si>
-    <t>Service Status</t>
-  </si>
-  <si>
-    <t>Service Date</t>
   </si>
   <si>
     <t>Technician Comment</t>
@@ -77,6 +71,12 @@
       </rPr>
       <t>solution@pestmanagements.in</t>
     </r>
+  </si>
+  <si>
+    <t>Visit Status</t>
+  </si>
+  <si>
+    <t>Visit Date</t>
   </si>
 </sst>
 </file>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,7 +686,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -697,7 +697,7 @@
     </row>
     <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -717,16 +717,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>